<commit_message>
Modificación consulta logs, implementación consulta historicos.
</commit_message>
<xml_diff>
--- a/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
+++ b/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91EDFFBC-7D6F-41D8-8B72-6AB5ACCA2929}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46879094-C6C1-42FA-B9AB-95E4A30770FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7485" xr2:uid="{68CBF942-DA0C-474A-8740-B976881B6C5B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7485" xr2:uid="{B0D352BF-2FEF-4D7D-A763-2A9E90A09630}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,18 +31,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t xml:space="preserve">Universidad Politécnica Salesiana </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>SISTEMA DE GESTIÓN DE INVENTARIOS Y TICKETING PARA SOPORTE TÉCNICO</t>
+  </si>
+  <si>
+    <t>Departamento de Laboratorios del ICC</t>
+  </si>
+  <si>
+    <t>Control de Inventario de Hardware y Software</t>
+  </si>
+  <si>
+    <t>Sede:</t>
+  </si>
+  <si>
+    <t>Fecha:</t>
+  </si>
+  <si>
+    <t>N° Equipos:</t>
+  </si>
+  <si>
+    <t>Laboratorio:</t>
+  </si>
+  <si>
+    <t>Quito, campus sur.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -57,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -65,15 +107,100 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{A1E74461-A6A6-408C-B834-C71AFDD0D62B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -93,45 +220,37 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="2" name="1 Imagen" descr="LOGO-UPS-300.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EE0AE84-CE59-4FA1-9998-9EDF660B234D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{813A1296-561F-49DB-9F61-82D6DA2BB4E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
+        <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="85725" y="0"/>
-          <a:ext cx="495300" cy="495300"/>
+          <a:off x="19050" y="76200"/>
+          <a:ext cx="1438275" cy="390525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -439,22 +558,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C10DECD-81EF-4CF6-AA17-1801986BC44F}">
-  <dimension ref="B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B7E2E6-F2E1-4330-9DDD-88EF45B10720}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C3:H3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implementación para reportes PDF y Excel para activos de TI.
</commit_message>
<xml_diff>
--- a/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
+++ b/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Source\Repos\DCICC.GestionInventarios\DCICC.GestionInventarios\DCICC.GestionInventarios\Reportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46879094-C6C1-42FA-B9AB-95E4A30770FF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9872F89E-7490-4311-B7BA-3A2E2AFD2821}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7485" xr2:uid="{B0D352BF-2FEF-4D7D-A763-2A9E90A09630}"/>
   </bookViews>
@@ -99,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -154,6 +154,74 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -164,29 +232,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -196,7 +244,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -217,18 +309,18 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1228725</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -239,7 +331,9 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr/>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
@@ -249,8 +343,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19050" y="76200"/>
-          <a:ext cx="1438275" cy="390525"/>
+          <a:off x="0" y="85725"/>
+          <a:ext cx="1228725" cy="380999"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -562,105 +656,110 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="H1" s="6"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="3" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="B7:H7"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Reportes PDF y Excel para activos, logs, maq virtuales y tickets.
</commit_message>
<xml_diff>
--- a/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
+++ b/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Source\Repos\DCICC.GestionInventarios\DCICC.GestionInventarios\DCICC.GestionInventarios\Reportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9872F89E-7490-4311-B7BA-3A2E2AFD2821}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0D4C8B-66BB-407E-9C53-6D74F6BBD1FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7485" xr2:uid="{B0D352BF-2FEF-4D7D-A763-2A9E90A09630}"/>
   </bookViews>
@@ -31,16 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>SISTEMA DE GESTIÓN DE INVENTARIOS Y TICKETING PARA SOPORTE TÉCNICO</t>
-  </si>
-  <si>
-    <t>Departamento de Laboratorios del ICC</t>
-  </si>
-  <si>
-    <t>Control de Inventario de Hardware y Software</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Sede:</t>
   </si>
@@ -53,15 +44,12 @@
   <si>
     <t>Laboratorio:</t>
   </si>
-  <si>
-    <t>Quito, campus sur.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,14 +70,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -99,7 +79,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -126,43 +106,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -187,37 +130,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -232,62 +144,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -314,13 +181,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1228725</xdr:colOff>
+      <xdr:colOff>1704975</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -343,8 +210,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="85725"/>
-          <a:ext cx="1228725" cy="380999"/>
+          <a:off x="0" y="38100"/>
+          <a:ext cx="1704975" cy="514350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -653,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B7E2E6-F2E1-4330-9DDD-88EF45B10720}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A3"/>
@@ -661,105 +528,42 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+    </row>
+    <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="14" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="17" t="s">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Corrección modificación de roles, usuarios en BD, reportes campos.
</commit_message>
<xml_diff>
--- a/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
+++ b/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Source\Repos\DCICC.GestionInventarios\DCICC.GestionInventarios\DCICC.GestionInventarios\Reportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0D4C8B-66BB-407E-9C53-6D74F6BBD1FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2C6099-91A2-40AB-8991-1534EDD52A94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7485" xr2:uid="{B0D352BF-2FEF-4D7D-A763-2A9E90A09630}"/>
   </bookViews>
@@ -31,18 +31,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Sede:</t>
+    <t>Laboratorio:</t>
+  </si>
+  <si>
+    <t>N° de Registros:</t>
   </si>
   <si>
     <t>Fecha:</t>
-  </si>
-  <si>
-    <t>N° Equipos:</t>
-  </si>
-  <si>
-    <t>Laboratorio:</t>
   </si>
 </sst>
 </file>
@@ -520,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B7E2E6-F2E1-4330-9DDD-88EF45B10720}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,22 +540,17 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrección imagen encabezado logo.
</commit_message>
<xml_diff>
--- a/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
+++ b/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Source\Repos\DCICC.GestionInventarios\DCICC.GestionInventarios\DCICC.GestionInventarios\Reportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2C6099-91A2-40AB-8991-1534EDD52A94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF64C38-67B1-46E9-968D-8646677AC580}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7485" xr2:uid="{B0D352BF-2FEF-4D7D-A763-2A9E90A09630}"/>
   </bookViews>
@@ -199,11 +199,10 @@
           <a:picLocks/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect t="-5866" b="-5866"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
@@ -520,7 +519,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrección dispose en imagen para reportes.
</commit_message>
<xml_diff>
--- a/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
+++ b/DCICC.GestionInventarios/DCICC.GestionInventarios/Reportes/PlantillaExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Source\Repos\DCICC.GestionInventarios\DCICC.GestionInventarios\DCICC.GestionInventarios\Reportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF64C38-67B1-46E9-968D-8646677AC580}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6954DAC-8F2C-4EE4-A0F1-9B45FA2A2A38}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7485" xr2:uid="{B0D352BF-2FEF-4D7D-A763-2A9E90A09630}"/>
   </bookViews>
@@ -169,54 +169,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1704975</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="1 Imagen" descr="LOGO-UPS-300.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{813A1296-561F-49DB-9F61-82D6DA2BB4E1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect t="-5866" b="-5866"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="38100"/>
-          <a:ext cx="1704975" cy="514350"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -558,6 +510,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>